<commit_message>
Added example UCUM units column to CHEM results template
</commit_message>
<xml_diff>
--- a/class_CHEM/results_template.xlsx
+++ b/class_CHEM/results_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32550" windowHeight="16395" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32550" windowHeight="16395"/>
   </bookViews>
   <sheets>
     <sheet name="group size &gt; 1" sheetId="1" r:id="rId1"/>
@@ -22,10 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -407,22 +403,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" customWidth="1"/>
-    <col min="13" max="13" width="86" customWidth="1"/>
-    <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" customWidth="1"/>
+    <col min="14" max="14" width="86" customWidth="1"/>
+    <col min="16" max="16" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -430,9 +426,9 @@
       <c r="A4" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H1 F1:F1048576 J1:J1048576 H3:H1048576">
+  <conditionalFormatting sqref="I1 G1:G1048576 K1:K1048576 I3:I1048576">
     <cfRule type="expression" dxfId="7" priority="4">
-      <formula>F1&lt;&gt;E1</formula>
+      <formula>G1&lt;&gt;F1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
@@ -440,12 +436,12 @@
       <formula>$B1=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="I2">
     <cfRule type="expression" dxfId="5" priority="2">
-      <formula>H2&lt;&gt;G2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
+      <formula>I2&lt;&gt;H2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="expression" dxfId="4" priority="1" stopIfTrue="1">
       <formula>$C1=""</formula>
     </cfRule>
@@ -458,31 +454,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" customWidth="1"/>
     <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" customWidth="1"/>
-    <col min="13" max="13" width="86" customWidth="1"/>
-    <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" customWidth="1"/>
+    <col min="14" max="14" width="86" customWidth="1"/>
+    <col min="16" max="16" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="H1 F1:F1048576 J1:J1048576 H3:H1048576">
+  <conditionalFormatting sqref="I1 G1:G1048576 K1:K1048576 I3:I1048576">
     <cfRule type="expression" dxfId="3" priority="6">
-      <formula>F1&lt;&gt;E1</formula>
+      <formula>G1&lt;&gt;F1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
@@ -490,12 +486,12 @@
       <formula>$B1=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="I2">
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>H2&lt;&gt;G2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
+      <formula>I2&lt;&gt;H2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>$C1=""</formula>
     </cfRule>

</xml_diff>

<commit_message>
Corrected which columns are hidden in CHEM template
</commit_message>
<xml_diff>
--- a/class_CHEM/results_template.xlsx
+++ b/class_CHEM/results_template.xlsx
@@ -403,7 +403,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -418,7 +421,8 @@
     <col min="12" max="12" width="11.42578125" customWidth="1"/>
     <col min="13" max="13" width="18.28515625" customWidth="1"/>
     <col min="14" max="14" width="86" customWidth="1"/>
-    <col min="16" max="16" width="0" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
+    <col min="17" max="17" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -455,7 +459,8 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,7 +476,8 @@
     <col min="12" max="12" width="11.42578125" customWidth="1"/>
     <col min="13" max="13" width="18.28515625" customWidth="1"/>
     <col min="14" max="14" width="86" customWidth="1"/>
-    <col min="16" max="16" width="0" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
+    <col min="17" max="17" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Implemented new approach for class CHEM and revised DRUG_TOX to share code and configuration with CHEM, because the two have almost the same processing
</commit_message>
<xml_diff>
--- a/class_CHEM/results_template.xlsx
+++ b/class_CHEM/results_template.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\project\loinc-equivalence-classes\class_CHEM\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="32550" windowHeight="16395"/>
   </bookViews>
@@ -16,12 +11,11 @@
     <sheet name="all groups" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -401,36 +395,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" customWidth="1"/>
     <col min="12" max="12" width="11.42578125" customWidth="1"/>
-    <col min="13" max="13" width="18.28515625" customWidth="1"/>
-    <col min="14" max="14" width="86" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" customWidth="1"/>
-    <col min="17" max="17" width="0" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="56.42578125" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" customWidth="1"/>
+    <col min="18" max="18" width="56.42578125" customWidth="1"/>
+    <col min="19" max="19" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I1 G1:G1048576 K1:K1048576 I3:I1048576">
+  <conditionalFormatting sqref="I1 G1:G1048576 K1:K1048576 I3:I1048576 M1:M1048576 O1:O1048576">
     <cfRule type="expression" dxfId="7" priority="4">
       <formula>G1&lt;&gt;F1</formula>
     </cfRule>
@@ -456,34 +472,58 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" customWidth="1"/>
     <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
     <col min="10" max="10" width="13.85546875" customWidth="1"/>
     <col min="11" max="11" width="14.5703125" customWidth="1"/>
     <col min="12" max="12" width="11.42578125" customWidth="1"/>
     <col min="13" max="13" width="18.28515625" customWidth="1"/>
-    <col min="14" max="14" width="86" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" customWidth="1"/>
-    <col min="17" max="17" width="0" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" customWidth="1"/>
+    <col min="16" max="16" width="49.140625" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" customWidth="1"/>
+    <col min="18" max="18" width="45.7109375" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="I1 G1:G1048576 K1:K1048576 I3:I1048576">
-    <cfRule type="expression" dxfId="3" priority="6">
+  <conditionalFormatting sqref="I1 G1:G1048576 K1:K1048576 I3:I1048576 M1:M1048576 O1:O1048576">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>G1&lt;&gt;F1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixes for SCALE in DrugTox & CHEM
</commit_message>
<xml_diff>
--- a/class_CHEM/results_template.xlsx
+++ b/class_CHEM/results_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32550" windowHeight="16395"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32550" windowHeight="16395" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="group size &gt; 1" sheetId="1" r:id="rId1"/>
@@ -395,11 +395,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" sqref="A1:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,18 +413,18 @@
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
     <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
     <col min="13" max="13" width="14.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="14" max="14" width="68.42578125" customWidth="1"/>
+    <col min="15" max="15" width="19.5703125" customWidth="1"/>
     <col min="16" max="16" width="56.42578125" customWidth="1"/>
-    <col min="17" max="17" width="11.85546875" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="56.42578125" customWidth="1"/>
     <col min="19" max="19" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -442,27 +442,25 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I1 G1:G1048576 K1:K1048576 I3:I1048576 M1:M1048576 O1:O1048576">
-    <cfRule type="expression" dxfId="7" priority="4">
+  <conditionalFormatting sqref="I1 G1:G1048576 I3:I1048576 M1:M1048576 K1:K1048576">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>G1&lt;&gt;F1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>$B1=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>I2&lt;&gt;H2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="expression" dxfId="4" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="I1:I1048576 K1:K1048576">
+    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
       <formula>$C1=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -474,9 +472,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,17 +488,17 @@
     <col min="9" max="9" width="11" customWidth="1"/>
     <col min="10" max="10" width="13.85546875" customWidth="1"/>
     <col min="11" max="11" width="14.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
     <col min="13" max="13" width="18.28515625" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" customWidth="1"/>
-    <col min="15" max="15" width="14.5703125" customWidth="1"/>
+    <col min="14" max="14" width="64.7109375" customWidth="1"/>
+    <col min="15" max="15" width="20.5703125" customWidth="1"/>
     <col min="16" max="16" width="49.140625" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="45.7109375" customWidth="1"/>
     <col min="19" max="19" width="14.42578125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -518,27 +516,25 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I1 G1:G1048576 K1:K1048576 I3:I1048576 M1:M1048576 O1:O1048576">
-    <cfRule type="expression" dxfId="3" priority="4">
+  <conditionalFormatting sqref="I1 G1:G2 M1:M2 K1:K2">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>G1&lt;&gt;F1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="expression" dxfId="2" priority="3">
+  <conditionalFormatting sqref="A1:A2">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>$B1=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>I2&lt;&gt;H2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="I1:I2 K1:K2">
+    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
       <formula>$C1=""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>